<commit_message>
20200629 CRE19-028  To enhance eHS(S) to cope with the IDEAS combo development 20200629 CRE19-021  To enhance the monthly report eHS(S)M0011 by adding 2 DHC data fields 20200629 INT20-0014 Fix unable to open invalidated PPP transaction 20200629 INT20-0019 Fix generate write-off for account deceased before 2009INT20-0020	Fix to 20200630 INT20-0020 reload JS file 20200702 INT20-0022 Fix IMMDValidation on IDEAS Combo
</commit_message>
<xml_diff>
--- a/EHS2019/EHS/ExcelGenerator/Template/eHSM0011-Voucher_Claim_DHC_Template.xlsx
+++ b/EHS2019/EHS/ExcelGenerator/Template/eHSM0011-Voucher_Claim_DHC_Template.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\EHS2015\ExcelGenerator\bin\Debug\Template\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="90" windowWidth="11475" windowHeight="6915"/>
   </bookViews>
@@ -12,12 +17,12 @@
     <sheet name="Remark" sheetId="3" r:id="rId3"/>
     <sheet name="Change History" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Sub Report ID</t>
   </si>
@@ -121,9 +126,6 @@
     <t xml:space="preserve">(c) Cumulative number of elders who have made use of vouchers for each service </t>
   </si>
   <si>
-    <t xml:space="preserve">(d) Cumulative number of elders who have ever made use of vouchers for District Health Centre related services </t>
-  </si>
-  <si>
     <t>(b) Cumulative amount of vouchers claimed ($)</t>
   </si>
   <si>
@@ -143,34 +145,54 @@
   </si>
   <si>
     <t>CRE19-006-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(e) Number of Service Providers eligible to make voucher claim for DHC-related services </t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>(f) Number of Service Provders who had made voucher claim for DHC-related services</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enhance DHC report</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>CRE19-021</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">(d) Cumulative number of elders who have ever made use of vouchers for District Health Centre related services (DHC-related services) </t>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -189,7 +211,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -225,6 +247,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -240,7 +269,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -264,6 +293,54 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -271,7 +348,9 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -280,7 +359,9 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -291,14 +372,77 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -306,8 +450,51 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -315,18 +502,7 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <left style="dotted">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -335,86 +511,9 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -443,7 +542,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
       <alignment vertical="center"/>
@@ -466,7 +565,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -482,111 +581,120 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -605,6 +713,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -653,7 +764,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -688,7 +799,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -903,14 +1014,14 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.28515625" style="9" customWidth="1"/>
     <col min="2" max="2" width="81.7109375" style="9" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -918,29 +1029,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
     </row>
-    <row r="5" spans="1:2" ht="15.75">
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="10"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -948,320 +1060,362 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q18"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="63.28515625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" style="13" customWidth="1"/>
-    <col min="3" max="16" width="10.7109375" style="13" customWidth="1"/>
-    <col min="17" max="17" width="20.5703125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" style="13" customWidth="1"/>
+    <col min="3" max="16" width="10.5703125" style="13" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" style="13" customWidth="1"/>
     <col min="18" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="12" customFormat="1" ht="15.75">
+    <row r="1" spans="1:17" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="str">
         <f>Content!A2 &amp;": "&amp;Content!B2</f>
         <v>eHS(S)M0011-01: Report of use of vouchers for District Health Centre related services</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75">
+    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="12" customFormat="1" ht="15.75">
-      <c r="A4" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" s="12" customFormat="1" ht="15.75"/>
-    <row r="6" spans="1:17" s="12" customFormat="1" ht="15.75"/>
-    <row r="7" spans="1:17" ht="15.75">
-      <c r="A7" s="45"/>
-      <c r="B7" s="47" t="s">
+    <row r="5" spans="1:17" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:17" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="25"/>
+      <c r="B7" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="47" t="s">
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="48"/>
-      <c r="H7" s="48"/>
-      <c r="I7" s="48"/>
-      <c r="J7" s="48"/>
-      <c r="K7" s="48"/>
-      <c r="L7" s="48"/>
-      <c r="M7" s="48"/>
-      <c r="N7" s="48"/>
-      <c r="O7" s="48"/>
-      <c r="P7" s="49"/>
-      <c r="Q7" s="43" t="s">
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="21" customFormat="1" ht="47.25">
-      <c r="A8" s="46"/>
-      <c r="B8" s="14" t="s">
+    <row r="8" spans="1:17" s="20" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="26"/>
+      <c r="B8" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="I8" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="15" t="s">
+      <c r="J8" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="K8" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="L8" s="15" t="s">
+      <c r="L8" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="15" t="s">
+      <c r="M8" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="N8" s="15" t="s">
+      <c r="N8" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="O8" s="15" t="s">
+      <c r="O8" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="P8" s="20" t="s">
+      <c r="P8" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="Q8" s="44"/>
-    </row>
-    <row r="9" spans="1:17" ht="33" customHeight="1">
-      <c r="A9" s="16" t="s">
+      <c r="Q8" s="24"/>
+    </row>
+    <row r="9" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="25"/>
-    </row>
-    <row r="10" spans="1:17" ht="15.75">
-      <c r="A10" s="17" t="s">
+      <c r="B9" s="41"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="47"/>
+      <c r="O9" s="47"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="31"/>
+    </row>
+    <row r="10" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="27"/>
-      <c r="O10" s="27"/>
-      <c r="P10" s="28"/>
-      <c r="Q10" s="29"/>
-    </row>
-    <row r="11" spans="1:17" ht="15.75">
-      <c r="A11" s="17" t="s">
+      <c r="B10" s="42"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
+      <c r="O10" s="48"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="33"/>
+    </row>
+    <row r="11" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="27"/>
-      <c r="P11" s="28"/>
-      <c r="Q11" s="29"/>
-    </row>
-    <row r="12" spans="1:17" ht="15.75">
-      <c r="A12" s="17" t="s">
+      <c r="B11" s="42"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="48"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="48"/>
+      <c r="N11" s="48"/>
+      <c r="O11" s="48"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="33"/>
+    </row>
+    <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="27"/>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="29"/>
-    </row>
-    <row r="13" spans="1:17" ht="15.75">
-      <c r="A13" s="17" t="s">
+      <c r="B12" s="42"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="48"/>
+      <c r="O12" s="48"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="33"/>
+    </row>
+    <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="28"/>
-      <c r="Q13" s="29"/>
-    </row>
-    <row r="14" spans="1:17" ht="15.75">
-      <c r="A14" s="18" t="s">
+      <c r="B13" s="42"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="48"/>
+      <c r="O13" s="48"/>
+      <c r="P13" s="32"/>
+      <c r="Q13" s="33"/>
+    </row>
+    <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="31"/>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="33"/>
-    </row>
-    <row r="15" spans="1:17" ht="31.5">
-      <c r="A15" s="19" t="s">
+      <c r="B14" s="43"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="49"/>
+      <c r="M14" s="49"/>
+      <c r="N14" s="49"/>
+      <c r="O14" s="49"/>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="35"/>
+    </row>
+    <row r="15" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="35"/>
-      <c r="P15" s="36"/>
-      <c r="Q15" s="37"/>
-    </row>
-    <row r="16" spans="1:17" ht="28.5" customHeight="1">
-      <c r="A16" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="35"/>
-      <c r="P16" s="36"/>
-      <c r="Q16" s="37"/>
-    </row>
-    <row r="17" spans="1:17" ht="31.5">
-      <c r="A17" s="19" t="s">
+      <c r="B15" s="44"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="50"/>
+      <c r="L15" s="50"/>
+      <c r="M15" s="50"/>
+      <c r="N15" s="50"/>
+      <c r="O15" s="50"/>
+      <c r="P15" s="37"/>
+      <c r="Q15" s="38"/>
+    </row>
+    <row r="16" spans="1:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="44"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="50"/>
+      <c r="L16" s="50"/>
+      <c r="M16" s="50"/>
+      <c r="N16" s="50"/>
+      <c r="O16" s="50"/>
+      <c r="P16" s="37"/>
+      <c r="Q16" s="38"/>
+    </row>
+    <row r="17" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="36"/>
-      <c r="Q17" s="37"/>
-    </row>
-    <row r="18" spans="1:17" ht="36" customHeight="1">
-      <c r="A18" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="39"/>
-      <c r="M18" s="39"/>
-      <c r="N18" s="39"/>
-      <c r="O18" s="39"/>
-      <c r="P18" s="40"/>
-      <c r="Q18" s="37"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="50"/>
+      <c r="L17" s="50"/>
+      <c r="M17" s="50"/>
+      <c r="N17" s="50"/>
+      <c r="O17" s="50"/>
+      <c r="P17" s="37"/>
+      <c r="Q17" s="38"/>
+    </row>
+    <row r="18" spans="1:17" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="45"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="51"/>
+      <c r="M18" s="51"/>
+      <c r="N18" s="51"/>
+      <c r="O18" s="51"/>
+      <c r="P18" s="39"/>
+      <c r="Q18" s="38"/>
+    </row>
+    <row r="19" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="44"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="50"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="50"/>
+      <c r="N19" s="50"/>
+      <c r="O19" s="50"/>
+      <c r="P19" s="36"/>
+      <c r="Q19" s="38"/>
+    </row>
+    <row r="20" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="43"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="50"/>
+      <c r="N20" s="50"/>
+      <c r="O20" s="50"/>
+      <c r="P20" s="36"/>
+      <c r="Q20" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1270,6 +1424,7 @@
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="F7:P7"/>
   </mergeCells>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1281,34 +1436,35 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" style="42" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" style="42" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="42"/>
+    <col min="1" max="1" width="29.85546875" style="22" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" style="22" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="41"/>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="41"/>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="41"/>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="21"/>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="21"/>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="21"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.85546875" style="9" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" style="9" customWidth="1"/>
@@ -1317,7 +1473,7 @@
     <col min="5" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1325,13 +1481,13 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75">
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -1345,21 +1501,36 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>1</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="8">
         <v>43727</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="8">
+        <v>44011</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
20210831 CRE21-008-01	To allow EHCP to choose make claims and generate reports and statistics for respective DHC and DHC Express - Phase 1 Sai Kung only
</commit_message>
<xml_diff>
--- a/EHS2019/EHS/ExcelGenerator/Template/eHSM0011-Voucher_Claim_DHC_Template.xlsx
+++ b/EHS2019/EHS/ExcelGenerator/Template/eHSM0011-Voucher_Claim_DHC_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Development\InternalChangeControl\2020\CRE20-006 (DHC Integration)\Front-end\ExcelGenerator\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ce5-fs01\ehs$\Development\InternalChangeControl\2021\CRE21-008 (DHC Express)\Front-end\ExcelGenerator\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,16 +16,17 @@
     <sheet name="01-All" sheetId="9" r:id="rId2"/>
     <sheet name="02-KT" sheetId="12" r:id="rId3"/>
     <sheet name="03-SSP" sheetId="13" r:id="rId4"/>
-    <sheet name="DHC Centre" sheetId="7" r:id="rId5"/>
-    <sheet name="Remark" sheetId="3" r:id="rId6"/>
-    <sheet name="Change History" sheetId="4" r:id="rId7"/>
+    <sheet name="04-SK" sheetId="14" r:id="rId5"/>
+    <sheet name="DHC Centre" sheetId="7" r:id="rId6"/>
+    <sheet name="Remark" sheetId="3" r:id="rId7"/>
+    <sheet name="Change History" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="67">
   <si>
     <t>Sub Report ID</t>
   </si>
@@ -218,6 +219,22 @@
   </si>
   <si>
     <t>Abbreviation</t>
+  </si>
+  <si>
+    <t>eHS(S)M0011-04</t>
+  </si>
+  <si>
+    <t>Report of use of vouchers for District Health Centre related services (Sai Kung)</t>
+  </si>
+  <si>
+    <t>CRE21-008</t>
+  </si>
+  <si>
+    <t>To generate reports and statistics for respective DHC and DHC Express</t>
+  </si>
+  <si>
+    <t>2021/08/31</t>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -225,27 +242,27 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -264,7 +281,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -302,7 +319,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -311,14 +328,14 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -698,7 +715,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
       <alignment vertical="center"/>
@@ -721,7 +738,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -821,7 +838,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -914,6 +931,27 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -949,9 +987,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1269,14 +1304,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.28515625" style="9" customWidth="1"/>
     <col min="2" max="2" width="81.7109375" style="9" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1284,7 +1319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>36</v>
       </c>
@@ -1292,7 +1327,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>42</v>
       </c>
@@ -1300,7 +1335,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>55</v>
       </c>
@@ -1308,15 +1343,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
     </row>
-    <row r="7" spans="1:2" ht="15.75">
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -1335,7 +1374,7 @@
   <sheetViews>
     <sheetView zoomScale="69" zoomScaleNormal="69" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="63.28515625" style="13" customWidth="1"/>
     <col min="2" max="16" width="10.5703125" style="13" customWidth="1"/>
@@ -1343,58 +1382,58 @@
     <col min="18" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="12" customFormat="1" ht="15.75">
+    <row r="1" spans="1:19" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="str">
         <f>Content!A2 &amp;": "&amp;Content!B2</f>
         <v>eHS(S)M0011-01: Report of use of vouchers for District Health Centre related services (All)</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15.75">
+    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="12" customFormat="1" ht="15.75">
+    <row r="4" spans="1:19" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="12" customFormat="1" ht="15.75"/>
-    <row r="6" spans="1:19" s="12" customFormat="1" ht="15.75"/>
-    <row r="7" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A7" s="81"/>
-      <c r="B7" s="84" t="s">
+    <row r="5" spans="1:19" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:19" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="88"/>
+      <c r="B7" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="85"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="85"/>
-      <c r="F7" s="85"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="84" t="s">
+      <c r="C7" s="92"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="92"/>
+      <c r="G7" s="93"/>
+      <c r="H7" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="85"/>
-      <c r="J7" s="85"/>
-      <c r="K7" s="85"/>
-      <c r="L7" s="85"/>
-      <c r="M7" s="85"/>
-      <c r="N7" s="85"/>
-      <c r="O7" s="85"/>
-      <c r="P7" s="85"/>
-      <c r="Q7" s="85"/>
-      <c r="R7" s="86"/>
-      <c r="S7" s="75" t="s">
+      <c r="I7" s="92"/>
+      <c r="J7" s="92"/>
+      <c r="K7" s="92"/>
+      <c r="L7" s="92"/>
+      <c r="M7" s="92"/>
+      <c r="N7" s="92"/>
+      <c r="O7" s="92"/>
+      <c r="P7" s="92"/>
+      <c r="Q7" s="92"/>
+      <c r="R7" s="93"/>
+      <c r="S7" s="82" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="18" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A8" s="82"/>
-      <c r="B8" s="78" t="s">
+    <row r="8" spans="1:19" s="18" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="89"/>
+      <c r="B8" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="79"/>
-      <c r="D8" s="80"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="87"/>
       <c r="E8" s="68"/>
       <c r="F8" s="68"/>
       <c r="G8" s="69"/>
@@ -1409,10 +1448,10 @@
       <c r="P8" s="68"/>
       <c r="Q8" s="68"/>
       <c r="R8" s="69"/>
-      <c r="S8" s="76"/>
-    </row>
-    <row r="9" spans="1:19" ht="33" customHeight="1">
-      <c r="A9" s="83"/>
+      <c r="S8" s="83"/>
+    </row>
+    <row r="9" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="90"/>
       <c r="B9" s="64" t="s">
         <v>9</v>
       </c>
@@ -1464,9 +1503,9 @@
       <c r="R9" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="S9" s="77"/>
-    </row>
-    <row r="10" spans="1:19" ht="31.5">
+      <c r="S9" s="84"/>
+    </row>
+    <row r="10" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>26</v>
       </c>
@@ -1489,7 +1528,7 @@
       <c r="R10" s="19"/>
       <c r="S10" s="20"/>
     </row>
-    <row r="11" spans="1:19" ht="15.75">
+    <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>27</v>
       </c>
@@ -1512,7 +1551,7 @@
       <c r="R11" s="21"/>
       <c r="S11" s="22"/>
     </row>
-    <row r="12" spans="1:19" ht="15.75">
+    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>28</v>
       </c>
@@ -1535,7 +1574,7 @@
       <c r="R12" s="21"/>
       <c r="S12" s="22"/>
     </row>
-    <row r="13" spans="1:19" ht="15.75">
+    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>29</v>
       </c>
@@ -1558,7 +1597,7 @@
       <c r="R13" s="21"/>
       <c r="S13" s="22"/>
     </row>
-    <row r="14" spans="1:19" ht="15.75">
+    <row r="14" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>30</v>
       </c>
@@ -1581,7 +1620,7 @@
       <c r="R14" s="21"/>
       <c r="S14" s="22"/>
     </row>
-    <row r="15" spans="1:19" ht="15.75">
+    <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>31</v>
       </c>
@@ -1604,7 +1643,7 @@
       <c r="R15" s="23"/>
       <c r="S15" s="24"/>
     </row>
-    <row r="16" spans="1:19" ht="28.5" customHeight="1">
+    <row r="16" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>32</v>
       </c>
@@ -1627,7 +1666,7 @@
       <c r="R16" s="26"/>
       <c r="S16" s="27"/>
     </row>
-    <row r="17" spans="1:19" ht="15.75">
+    <row r="17" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>33</v>
       </c>
@@ -1650,7 +1689,7 @@
       <c r="R17" s="26"/>
       <c r="S17" s="27"/>
     </row>
-    <row r="18" spans="1:19" ht="39.75" customHeight="1">
+    <row r="18" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>57</v>
       </c>
@@ -1673,7 +1712,7 @@
       <c r="R18" s="26"/>
       <c r="S18" s="27"/>
     </row>
-    <row r="19" spans="1:19" ht="47.25">
+    <row r="19" spans="1:19" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>58</v>
       </c>
@@ -1696,7 +1735,7 @@
       <c r="R19" s="28"/>
       <c r="S19" s="27"/>
     </row>
-    <row r="20" spans="1:19" ht="31.5">
+    <row r="20" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>59</v>
       </c>
@@ -1719,7 +1758,7 @@
       <c r="R20" s="25"/>
       <c r="S20" s="27"/>
     </row>
-    <row r="21" spans="1:19" ht="31.5">
+    <row r="21" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>60</v>
       </c>
@@ -1742,8 +1781,8 @@
       <c r="R21" s="25"/>
       <c r="S21" s="27"/>
     </row>
-    <row r="24" spans="1:19">
-      <c r="A24" s="87" t="s">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="80" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1755,6 +1794,7 @@
     <mergeCell ref="B7:G7"/>
     <mergeCell ref="H7:R7"/>
   </mergeCells>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1766,7 +1806,7 @@
   <sheetViews>
     <sheetView zoomScale="69" zoomScaleNormal="69" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="63.28515625" style="13" customWidth="1"/>
     <col min="2" max="16" width="10.5703125" style="13" customWidth="1"/>
@@ -1774,58 +1814,58 @@
     <col min="18" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="12" customFormat="1" ht="15.75">
+    <row r="1" spans="1:19" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="str">
         <f>Content!A3 &amp;": "&amp;Content!B3</f>
         <v>eHS(S)M0011-02: Report of use of vouchers for District Health Centre related services (Kwai Tsing)</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15.75">
+    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="12" customFormat="1" ht="15.75">
+    <row r="4" spans="1:19" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="12" customFormat="1" ht="15.75"/>
-    <row r="6" spans="1:19" s="12" customFormat="1" ht="15.75"/>
-    <row r="7" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A7" s="81"/>
-      <c r="B7" s="84" t="s">
+    <row r="5" spans="1:19" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:19" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="88"/>
+      <c r="B7" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="85"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="85"/>
-      <c r="F7" s="85"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="84" t="s">
+      <c r="C7" s="92"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="92"/>
+      <c r="G7" s="93"/>
+      <c r="H7" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="85"/>
-      <c r="J7" s="85"/>
-      <c r="K7" s="85"/>
-      <c r="L7" s="85"/>
-      <c r="M7" s="85"/>
-      <c r="N7" s="85"/>
-      <c r="O7" s="85"/>
-      <c r="P7" s="85"/>
-      <c r="Q7" s="85"/>
-      <c r="R7" s="86"/>
-      <c r="S7" s="75" t="s">
+      <c r="I7" s="92"/>
+      <c r="J7" s="92"/>
+      <c r="K7" s="92"/>
+      <c r="L7" s="92"/>
+      <c r="M7" s="92"/>
+      <c r="N7" s="92"/>
+      <c r="O7" s="92"/>
+      <c r="P7" s="92"/>
+      <c r="Q7" s="92"/>
+      <c r="R7" s="93"/>
+      <c r="S7" s="82" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="18" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A8" s="82"/>
-      <c r="B8" s="78" t="s">
+    <row r="8" spans="1:19" s="18" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="89"/>
+      <c r="B8" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="79"/>
-      <c r="D8" s="80"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="87"/>
       <c r="E8" s="73"/>
       <c r="F8" s="73"/>
       <c r="G8" s="74"/>
@@ -1840,10 +1880,10 @@
       <c r="P8" s="73"/>
       <c r="Q8" s="73"/>
       <c r="R8" s="74"/>
-      <c r="S8" s="76"/>
-    </row>
-    <row r="9" spans="1:19" ht="33" customHeight="1">
-      <c r="A9" s="83"/>
+      <c r="S8" s="83"/>
+    </row>
+    <row r="9" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="90"/>
       <c r="B9" s="64" t="s">
         <v>9</v>
       </c>
@@ -1895,9 +1935,9 @@
       <c r="R9" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="S9" s="77"/>
-    </row>
-    <row r="10" spans="1:19" ht="31.5">
+      <c r="S9" s="84"/>
+    </row>
+    <row r="10" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>26</v>
       </c>
@@ -1920,7 +1960,7 @@
       <c r="R10" s="19"/>
       <c r="S10" s="20"/>
     </row>
-    <row r="11" spans="1:19" ht="15.75">
+    <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>27</v>
       </c>
@@ -1943,7 +1983,7 @@
       <c r="R11" s="21"/>
       <c r="S11" s="22"/>
     </row>
-    <row r="12" spans="1:19" ht="15.75">
+    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>28</v>
       </c>
@@ -1966,7 +2006,7 @@
       <c r="R12" s="21"/>
       <c r="S12" s="22"/>
     </row>
-    <row r="13" spans="1:19" ht="15.75">
+    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>29</v>
       </c>
@@ -1989,7 +2029,7 @@
       <c r="R13" s="21"/>
       <c r="S13" s="22"/>
     </row>
-    <row r="14" spans="1:19" ht="15.75">
+    <row r="14" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>30</v>
       </c>
@@ -2012,7 +2052,7 @@
       <c r="R14" s="21"/>
       <c r="S14" s="22"/>
     </row>
-    <row r="15" spans="1:19" ht="15.75">
+    <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>31</v>
       </c>
@@ -2035,7 +2075,7 @@
       <c r="R15" s="23"/>
       <c r="S15" s="24"/>
     </row>
-    <row r="16" spans="1:19" ht="28.5" customHeight="1">
+    <row r="16" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>32</v>
       </c>
@@ -2058,7 +2098,7 @@
       <c r="R16" s="26"/>
       <c r="S16" s="27"/>
     </row>
-    <row r="17" spans="1:19" ht="15.75">
+    <row r="17" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>33</v>
       </c>
@@ -2081,7 +2121,7 @@
       <c r="R17" s="26"/>
       <c r="S17" s="27"/>
     </row>
-    <row r="18" spans="1:19" ht="39.75" customHeight="1">
+    <row r="18" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>57</v>
       </c>
@@ -2104,7 +2144,7 @@
       <c r="R18" s="26"/>
       <c r="S18" s="27"/>
     </row>
-    <row r="19" spans="1:19" ht="47.25">
+    <row r="19" spans="1:19" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>58</v>
       </c>
@@ -2127,7 +2167,7 @@
       <c r="R19" s="28"/>
       <c r="S19" s="27"/>
     </row>
-    <row r="20" spans="1:19" ht="31.5">
+    <row r="20" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>59</v>
       </c>
@@ -2150,7 +2190,7 @@
       <c r="R20" s="25"/>
       <c r="S20" s="27"/>
     </row>
-    <row r="21" spans="1:19" ht="31.5">
+    <row r="21" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>60</v>
       </c>
@@ -2173,8 +2213,8 @@
       <c r="R21" s="25"/>
       <c r="S21" s="27"/>
     </row>
-    <row r="24" spans="1:19">
-      <c r="A24" s="87" t="s">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="80" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2186,6 +2226,7 @@
     <mergeCell ref="S7:S9"/>
     <mergeCell ref="B8:D8"/>
   </mergeCells>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2197,7 +2238,7 @@
   <sheetViews>
     <sheetView zoomScale="69" zoomScaleNormal="69" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="63.28515625" style="13" customWidth="1"/>
     <col min="2" max="16" width="10.5703125" style="13" customWidth="1"/>
@@ -2205,58 +2246,58 @@
     <col min="18" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="12" customFormat="1" ht="15.75">
+    <row r="1" spans="1:19" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="str">
         <f>Content!A4 &amp;": "&amp;Content!B4</f>
         <v>eHS(S)M0011-03: Report of use of vouchers for District Health Centre related services (Sham Shui Po)</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15.75">
+    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="12" customFormat="1" ht="15.75">
+    <row r="4" spans="1:19" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="12" customFormat="1" ht="15.75"/>
-    <row r="6" spans="1:19" s="12" customFormat="1" ht="15.75"/>
-    <row r="7" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A7" s="81"/>
-      <c r="B7" s="84" t="s">
+    <row r="5" spans="1:19" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:19" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="88"/>
+      <c r="B7" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="85"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="85"/>
-      <c r="F7" s="85"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="84" t="s">
+      <c r="C7" s="92"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="92"/>
+      <c r="G7" s="93"/>
+      <c r="H7" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="85"/>
-      <c r="J7" s="85"/>
-      <c r="K7" s="85"/>
-      <c r="L7" s="85"/>
-      <c r="M7" s="85"/>
-      <c r="N7" s="85"/>
-      <c r="O7" s="85"/>
-      <c r="P7" s="85"/>
-      <c r="Q7" s="85"/>
-      <c r="R7" s="86"/>
-      <c r="S7" s="75" t="s">
+      <c r="I7" s="92"/>
+      <c r="J7" s="92"/>
+      <c r="K7" s="92"/>
+      <c r="L7" s="92"/>
+      <c r="M7" s="92"/>
+      <c r="N7" s="92"/>
+      <c r="O7" s="92"/>
+      <c r="P7" s="92"/>
+      <c r="Q7" s="92"/>
+      <c r="R7" s="93"/>
+      <c r="S7" s="82" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="18" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A8" s="82"/>
-      <c r="B8" s="78" t="s">
+    <row r="8" spans="1:19" s="18" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="89"/>
+      <c r="B8" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="79"/>
-      <c r="D8" s="80"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="87"/>
       <c r="E8" s="73"/>
       <c r="F8" s="73"/>
       <c r="G8" s="74"/>
@@ -2271,10 +2312,10 @@
       <c r="P8" s="73"/>
       <c r="Q8" s="73"/>
       <c r="R8" s="74"/>
-      <c r="S8" s="76"/>
-    </row>
-    <row r="9" spans="1:19" ht="33" customHeight="1">
-      <c r="A9" s="83"/>
+      <c r="S8" s="83"/>
+    </row>
+    <row r="9" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="90"/>
       <c r="B9" s="64" t="s">
         <v>9</v>
       </c>
@@ -2326,9 +2367,9 @@
       <c r="R9" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="S9" s="77"/>
-    </row>
-    <row r="10" spans="1:19" ht="31.5">
+      <c r="S9" s="84"/>
+    </row>
+    <row r="10" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>26</v>
       </c>
@@ -2351,7 +2392,7 @@
       <c r="R10" s="19"/>
       <c r="S10" s="20"/>
     </row>
-    <row r="11" spans="1:19" ht="15.75">
+    <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>27</v>
       </c>
@@ -2374,7 +2415,7 @@
       <c r="R11" s="21"/>
       <c r="S11" s="22"/>
     </row>
-    <row r="12" spans="1:19" ht="15.75">
+    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>28</v>
       </c>
@@ -2397,7 +2438,7 @@
       <c r="R12" s="21"/>
       <c r="S12" s="22"/>
     </row>
-    <row r="13" spans="1:19" ht="15.75">
+    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>29</v>
       </c>
@@ -2420,7 +2461,7 @@
       <c r="R13" s="21"/>
       <c r="S13" s="22"/>
     </row>
-    <row r="14" spans="1:19" ht="15.75">
+    <row r="14" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>30</v>
       </c>
@@ -2443,7 +2484,7 @@
       <c r="R14" s="21"/>
       <c r="S14" s="22"/>
     </row>
-    <row r="15" spans="1:19" ht="15.75">
+    <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>31</v>
       </c>
@@ -2466,7 +2507,7 @@
       <c r="R15" s="23"/>
       <c r="S15" s="24"/>
     </row>
-    <row r="16" spans="1:19" ht="28.5" customHeight="1">
+    <row r="16" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>32</v>
       </c>
@@ -2489,7 +2530,7 @@
       <c r="R16" s="26"/>
       <c r="S16" s="27"/>
     </row>
-    <row r="17" spans="1:19" ht="15.75">
+    <row r="17" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>33</v>
       </c>
@@ -2512,7 +2553,7 @@
       <c r="R17" s="26"/>
       <c r="S17" s="27"/>
     </row>
-    <row r="18" spans="1:19" ht="39.75" customHeight="1">
+    <row r="18" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>57</v>
       </c>
@@ -2535,7 +2576,7 @@
       <c r="R18" s="26"/>
       <c r="S18" s="27"/>
     </row>
-    <row r="19" spans="1:19" ht="47.25">
+    <row r="19" spans="1:19" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>58</v>
       </c>
@@ -2558,7 +2599,7 @@
       <c r="R19" s="28"/>
       <c r="S19" s="27"/>
     </row>
-    <row r="20" spans="1:19" ht="31.5">
+    <row r="20" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>59</v>
       </c>
@@ -2581,7 +2622,7 @@
       <c r="R20" s="25"/>
       <c r="S20" s="27"/>
     </row>
-    <row r="21" spans="1:19" ht="31.5">
+    <row r="21" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>60</v>
       </c>
@@ -2604,8 +2645,8 @@
       <c r="R21" s="25"/>
       <c r="S21" s="27"/>
     </row>
-    <row r="24" spans="1:19">
-      <c r="A24" s="87" t="s">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="80" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2617,6 +2658,7 @@
     <mergeCell ref="S7:S9"/>
     <mergeCell ref="B8:D8"/>
   </mergeCells>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2624,11 +2666,443 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S24"/>
+  <sheetViews>
+    <sheetView zoomScale="69" zoomScaleNormal="69" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="63.28515625" style="13" customWidth="1"/>
+    <col min="2" max="16" width="10.5703125" style="13" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" style="13" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="str">
+        <f>Content!A5 &amp;": "&amp;Content!B5</f>
+        <v>eHS(S)M0011-04: Report of use of vouchers for District Health Centre related services (Sai Kung)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:19" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="88"/>
+      <c r="B7" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="92"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="92"/>
+      <c r="G7" s="93"/>
+      <c r="H7" s="91" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="92"/>
+      <c r="J7" s="92"/>
+      <c r="K7" s="92"/>
+      <c r="L7" s="92"/>
+      <c r="M7" s="92"/>
+      <c r="N7" s="92"/>
+      <c r="O7" s="92"/>
+      <c r="P7" s="92"/>
+      <c r="Q7" s="92"/>
+      <c r="R7" s="93"/>
+      <c r="S7" s="82" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" s="18" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="89"/>
+      <c r="B8" s="85" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="86"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="78"/>
+      <c r="F8" s="78"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="77"/>
+      <c r="I8" s="78"/>
+      <c r="J8" s="78"/>
+      <c r="K8" s="78"/>
+      <c r="L8" s="78"/>
+      <c r="M8" s="78"/>
+      <c r="N8" s="78"/>
+      <c r="O8" s="78"/>
+      <c r="P8" s="78"/>
+      <c r="Q8" s="78"/>
+      <c r="R8" s="79"/>
+      <c r="S8" s="83"/>
+    </row>
+    <row r="9" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="90"/>
+      <c r="B9" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="62" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="75" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="M9" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="N9" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="O9" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="P9" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q9" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="R9" s="76" t="s">
+        <v>22</v>
+      </c>
+      <c r="S9" s="84"/>
+    </row>
+    <row r="10" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="30"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="36"/>
+      <c r="O10" s="36"/>
+      <c r="P10" s="36"/>
+      <c r="Q10" s="36"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="20"/>
+    </row>
+    <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="31"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="37"/>
+      <c r="N11" s="37"/>
+      <c r="O11" s="37"/>
+      <c r="P11" s="37"/>
+      <c r="Q11" s="37"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="22"/>
+    </row>
+    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="31"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="37"/>
+      <c r="P12" s="37"/>
+      <c r="Q12" s="37"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="22"/>
+    </row>
+    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="31"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="37"/>
+      <c r="Q13" s="37"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="22"/>
+    </row>
+    <row r="14" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="31"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="37"/>
+      <c r="P14" s="37"/>
+      <c r="Q14" s="37"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="22"/>
+    </row>
+    <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="32"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="38"/>
+      <c r="R15" s="23"/>
+      <c r="S15" s="24"/>
+    </row>
+    <row r="16" spans="1:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="33"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="39"/>
+      <c r="P16" s="39"/>
+      <c r="Q16" s="39"/>
+      <c r="R16" s="26"/>
+      <c r="S16" s="27"/>
+    </row>
+    <row r="17" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="33"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="39"/>
+      <c r="L17" s="39"/>
+      <c r="M17" s="39"/>
+      <c r="N17" s="39"/>
+      <c r="O17" s="39"/>
+      <c r="P17" s="39"/>
+      <c r="Q17" s="39"/>
+      <c r="R17" s="26"/>
+      <c r="S17" s="27"/>
+    </row>
+    <row r="18" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="33"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="39"/>
+      <c r="M18" s="39"/>
+      <c r="N18" s="39"/>
+      <c r="O18" s="39"/>
+      <c r="P18" s="39"/>
+      <c r="Q18" s="39"/>
+      <c r="R18" s="26"/>
+      <c r="S18" s="27"/>
+    </row>
+    <row r="19" spans="1:19" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="34"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="40"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="40"/>
+      <c r="Q19" s="40"/>
+      <c r="R19" s="28"/>
+      <c r="S19" s="27"/>
+    </row>
+    <row r="20" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="33"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="39"/>
+      <c r="O20" s="39"/>
+      <c r="P20" s="39"/>
+      <c r="Q20" s="39"/>
+      <c r="R20" s="25"/>
+      <c r="S20" s="27"/>
+    </row>
+    <row r="21" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="32"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="39"/>
+      <c r="O21" s="39"/>
+      <c r="P21" s="39"/>
+      <c r="Q21" s="39"/>
+      <c r="R21" s="25"/>
+      <c r="S21" s="27"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="80" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="H7:R7"/>
+    <mergeCell ref="S7:S9"/>
+    <mergeCell ref="B8:D8"/>
+  </mergeCells>
+  <phoneticPr fontId="11" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.5703125" customWidth="1"/>
     <col min="2" max="3" width="13.85546875" customWidth="1"/>
@@ -2636,7 +3110,7 @@
     <col min="5" max="5" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
         <v>53</v>
       </c>
@@ -2645,14 +3119,14 @@
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
     </row>
-    <row r="3" spans="1:5" ht="15.75">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="44" t="s">
         <v>45</v>
       </c>
@@ -2669,7 +3143,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
         <v>50</v>
       </c>
@@ -2686,269 +3160,270 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="50"/>
       <c r="D5" s="50"/>
       <c r="E5" s="50"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="50"/>
       <c r="D6" s="50"/>
       <c r="E6" s="50"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="50"/>
       <c r="D7" s="50"/>
       <c r="E7" s="50"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="50"/>
       <c r="D8" s="50"/>
       <c r="E8" s="50"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="50"/>
       <c r="D9" s="50"/>
       <c r="E9" s="50"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="50"/>
       <c r="D10" s="50"/>
       <c r="E10" s="50"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="50"/>
       <c r="D11" s="50"/>
       <c r="E11" s="50"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="50"/>
       <c r="D12" s="50"/>
       <c r="E12" s="50"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="50"/>
       <c r="D13" s="50"/>
       <c r="E13" s="50"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="50"/>
       <c r="D14" s="50"/>
       <c r="E14" s="50"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="50"/>
       <c r="D15" s="50"/>
       <c r="E15" s="50"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="50"/>
       <c r="D16" s="50"/>
       <c r="E16" s="50"/>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="50"/>
       <c r="D17" s="50"/>
       <c r="E17" s="50"/>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="50"/>
       <c r="D18" s="50"/>
       <c r="E18" s="50"/>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="50"/>
       <c r="D19" s="50"/>
       <c r="E19" s="50"/>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="50"/>
       <c r="D20" s="50"/>
       <c r="E20" s="50"/>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="50"/>
       <c r="D21" s="50"/>
       <c r="E21" s="50"/>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="50"/>
       <c r="D22" s="50"/>
       <c r="E22" s="50"/>
     </row>
-    <row r="23" spans="2:5">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="50"/>
       <c r="D23" s="50"/>
       <c r="E23" s="50"/>
     </row>
-    <row r="24" spans="2:5">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="50"/>
       <c r="D24" s="50"/>
       <c r="E24" s="50"/>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="50"/>
       <c r="D25" s="50"/>
       <c r="E25" s="50"/>
     </row>
-    <row r="26" spans="2:5">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="50"/>
       <c r="D26" s="50"/>
       <c r="E26" s="50"/>
     </row>
-    <row r="27" spans="2:5">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="50"/>
       <c r="D27" s="50"/>
       <c r="E27" s="50"/>
     </row>
-    <row r="28" spans="2:5">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="50"/>
       <c r="D28" s="50"/>
       <c r="E28" s="50"/>
     </row>
-    <row r="29" spans="2:5">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="50"/>
       <c r="D29" s="50"/>
       <c r="E29" s="50"/>
     </row>
-    <row r="30" spans="2:5">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="50"/>
       <c r="D30" s="50"/>
       <c r="E30" s="50"/>
     </row>
-    <row r="31" spans="2:5">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="50"/>
       <c r="D31" s="50"/>
       <c r="E31" s="50"/>
     </row>
-    <row r="32" spans="2:5">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="50"/>
       <c r="D32" s="50"/>
       <c r="E32" s="50"/>
     </row>
-    <row r="33" spans="2:5">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="50"/>
       <c r="D33" s="50"/>
       <c r="E33" s="50"/>
     </row>
-    <row r="34" spans="2:5">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="50"/>
       <c r="D34" s="50"/>
       <c r="E34" s="50"/>
     </row>
-    <row r="35" spans="2:5">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="50"/>
       <c r="D35" s="50"/>
       <c r="E35" s="50"/>
     </row>
-    <row r="36" spans="2:5">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="50"/>
       <c r="D36" s="50"/>
       <c r="E36" s="50"/>
     </row>
-    <row r="37" spans="2:5">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="50"/>
     </row>
-    <row r="38" spans="2:5">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="50"/>
     </row>
-    <row r="39" spans="2:5">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="50"/>
     </row>
-    <row r="40" spans="2:5">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="50"/>
     </row>
-    <row r="41" spans="2:5">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="50"/>
     </row>
-    <row r="42" spans="2:5">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="50"/>
     </row>
-    <row r="43" spans="2:5">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="50"/>
     </row>
-    <row r="44" spans="2:5">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="50"/>
     </row>
-    <row r="45" spans="2:5">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="50"/>
     </row>
-    <row r="46" spans="2:5">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="50"/>
     </row>
-    <row r="47" spans="2:5">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="50"/>
     </row>
-    <row r="48" spans="2:5">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="50"/>
     </row>
-    <row r="49" spans="2:2">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="50"/>
     </row>
-    <row r="50" spans="2:2">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="50"/>
     </row>
-    <row r="51" spans="2:2">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="50"/>
     </row>
-    <row r="52" spans="2:2">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" s="50"/>
     </row>
-    <row r="53" spans="2:2">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" s="50"/>
     </row>
-    <row r="54" spans="2:2">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" s="50"/>
     </row>
-    <row r="55" spans="2:2">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" s="50"/>
     </row>
-    <row r="56" spans="2:2">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" s="50"/>
     </row>
-    <row r="57" spans="2:2">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" s="50"/>
     </row>
-    <row r="58" spans="2:2">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" s="50"/>
     </row>
-    <row r="59" spans="2:2">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" s="50"/>
     </row>
-    <row r="60" spans="2:2">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="50"/>
     </row>
-    <row r="61" spans="2:2">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" s="50"/>
     </row>
-    <row r="62" spans="2:2">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" s="50"/>
     </row>
-    <row r="63" spans="2:2">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" s="50"/>
     </row>
-    <row r="64" spans="2:2">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" s="50"/>
     </row>
-    <row r="65" spans="2:2">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="50"/>
     </row>
-    <row r="66" spans="2:2">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="50"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.85546875" customWidth="1"/>
     <col min="2" max="2" width="31.7109375" customWidth="1"/>
@@ -2959,13 +3434,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.85546875" style="9" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" style="9" customWidth="1"/>
@@ -2974,7 +3449,7 @@
     <col min="5" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -2982,13 +3457,13 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75">
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -3002,7 +3477,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -3016,7 +3491,7 @@
         <v>43727</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>2</v>
       </c>
@@ -3030,7 +3505,7 @@
         <v>44011</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="43">
         <v>3</v>
       </c>
@@ -3042,6 +3517,20 @@
       </c>
       <c r="D6" s="42">
         <v>44364</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="9">
+        <v>4</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="81" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20220428 CRS22-001	To update M0011 in light of new corporate accounts created for DHC express
</commit_message>
<xml_diff>
--- a/EHS2019/EHS/ExcelGenerator/Template/eHSM0011-Voucher_Claim_DHC_Template.xlsx
+++ b/EHS2019/EHS/ExcelGenerator/Template/eHSM0011-Voucher_Claim_DHC_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ce5-fs01\ehs$\Development\InternalChangeControl\2021\CRE21-008 (DHC Express)\Front-end (Phase 2 other districts)\ExcelGenerator\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ehp9-fs1\ehs$\Development\InternalChangeControl\2022\CRS22-001 (Update DHC eHSM0011)\Front-end\ExcelGenerator\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
     <sheet name="05-YTM" sheetId="15" r:id="rId6"/>
     <sheet name="06-KLC" sheetId="16" r:id="rId7"/>
     <sheet name="07-WC" sheetId="17" r:id="rId8"/>
-    <sheet name="08-KT" sheetId="18" r:id="rId9"/>
+    <sheet name="08-KwT" sheetId="18" r:id="rId9"/>
     <sheet name="09-TP" sheetId="19" r:id="rId10"/>
     <sheet name="10-ILD" sheetId="20" r:id="rId11"/>
     <sheet name="11-NTH" sheetId="21" r:id="rId12"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="91">
   <si>
     <t>Sub Report ID</t>
   </si>
@@ -311,6 +311,14 @@
   </si>
   <si>
     <t>2021/09/28</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>CRS22-001</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>To update M0011 in light of new corporate accounts created for DHC express</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
@@ -4487,9 +4495,11 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4596,6 +4606,20 @@
       </c>
       <c r="D8" s="81" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="42">
+        <v>44679</v>
       </c>
     </row>
   </sheetData>

</xml_diff>